<commit_message>
chore: add seeder account
</commit_message>
<xml_diff>
--- a/prisma/seeder/data.xlsx
+++ b/prisma/seeder/data.xlsx
@@ -4,17 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="132" yWindow="588" windowWidth="22716" windowHeight="8676"/>
+    <workbookView xWindow="132" yWindow="588" windowWidth="22716" windowHeight="8676" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="account" sheetId="6" r:id="rId1"/>
+    <sheet name="category" sheetId="7" r:id="rId2"/>
+    <sheet name="content" sheetId="8" r:id="rId3"/>
+    <sheet name="listContent" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>email</t>
   </si>
@@ -25,15 +28,6 @@
     <t>role</t>
   </si>
   <si>
-    <t>createdAt</t>
-  </si>
-  <si>
-    <t>updatedAt</t>
-  </si>
-  <si>
-    <t>$2b$10$4vzMK0mWW/eKo5UgDwKIB.XoAPQqPkE/mmq6V6g0cTCwL6TTRQnJW</t>
-  </si>
-  <si>
     <t>admin@gmail.com</t>
   </si>
   <si>
@@ -59,6 +53,99 @@
   </si>
   <si>
     <t>User</t>
+  </si>
+  <si>
+    <t>fullName</t>
+  </si>
+  <si>
+    <t>Fulan</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>081234567890</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Category 1</t>
+  </si>
+  <si>
+    <t>Category 2</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>creteBy</t>
+  </si>
+  <si>
+    <t>contentId</t>
+  </si>
+  <si>
+    <t>categoryId</t>
+  </si>
+  <si>
+    <t>createBy</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>categoryName</t>
+  </si>
+  <si>
+    <t>contentTitle</t>
+  </si>
+  <si>
+    <t>https://via.placeholder.com/150</t>
+  </si>
+  <si>
+    <t>Content 1</t>
+  </si>
+  <si>
+    <t>Content 2</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t>Description Content 1</t>
+  </si>
+  <si>
+    <t>Description Content 2</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=123456</t>
+  </si>
+  <si>
+    <t>081234567891</t>
   </si>
 </sst>
 </file>
@@ -82,12 +169,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -103,11 +196,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -445,105 +539,391 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.69921875" customWidth="1"/>
-    <col min="2" max="2" width="25.5" customWidth="1"/>
-    <col min="3" max="3" width="6.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.19921875" customWidth="1"/>
-    <col min="6" max="6" width="7.296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.69921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="15.69921875" customWidth="1"/>
+    <col min="6" max="6" width="25.5" customWidth="1"/>
+    <col min="7" max="7" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.19921875" customWidth="1"/>
+    <col min="10" max="10" width="7.296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1">
+        <v>123456</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1">
+        <v>123456</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.796875" customWidth="1"/>
+    <col min="2" max="2" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2">
+        <v>100000</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
+      <c r="B3" t="s">
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>8</v>
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3">
+        <v>100000</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.09765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <f>VLOOKUP(A2,content!A:D,4,0)</f>
+        <v>Content 1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <f>VLOOKUP(C2,category!A:B,2,0)</f>
+        <v>Category 1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="str">
+        <f>VLOOKUP(A3,content!A:D,4,0)</f>
+        <v>Content 1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="str">
+        <f>VLOOKUP(C3,category!A:B,2,0)</f>
+        <v>Category 2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="str">
+        <f>VLOOKUP(A4,content!A:D,4,0)</f>
+        <v>Content 2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="str">
+        <f>VLOOKUP(C4,category!A:B,2,0)</f>
+        <v>Category 1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
chore: add content seeder
</commit_message>
<xml_diff>
--- a/prisma/seeder/data.xlsx
+++ b/prisma/seeder/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="132" yWindow="588" windowWidth="22716" windowHeight="8676" activeTab="1"/>
+    <workbookView xWindow="132" yWindow="588" windowWidth="22716" windowHeight="8676" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="account" sheetId="6" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>email</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>price</t>
-  </si>
-  <si>
-    <t>creteBy</t>
   </si>
   <si>
     <t>contentId</t>
@@ -560,7 +557,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -640,7 +637,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
@@ -677,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -690,7 +687,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
@@ -731,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -742,7 +739,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
         <v>21</v>
@@ -763,7 +760,7 @@
         <v>26</v>
       </c>
       <c r="H1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
@@ -774,19 +771,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
         <v>34</v>
       </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2">
         <v>100000</v>
@@ -804,19 +801,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s">
         <v>40</v>
-      </c>
-      <c r="F3" t="s">
-        <v>41</v>
       </c>
       <c r="G3">
         <v>100000</v>
@@ -850,19 +847,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
         <v>29</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
chore: add seeder category and contentCategory
</commit_message>
<xml_diff>
--- a/prisma/seeder/data.xlsx
+++ b/prisma/seeder/data.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="132" yWindow="588" windowWidth="22716" windowHeight="8676" activeTab="2"/>
+    <workbookView xWindow="132" yWindow="588" windowWidth="22716" windowHeight="8676" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="account" sheetId="6" r:id="rId1"/>
     <sheet name="category" sheetId="7" r:id="rId2"/>
     <sheet name="content" sheetId="8" r:id="rId3"/>
-    <sheet name="listContent" sheetId="9" r:id="rId4"/>
+    <sheet name="contentCategory" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -675,7 +675,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -728,7 +728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -834,7 +834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
chore: update content seeder
</commit_message>
<xml_diff>
--- a/prisma/seeder/data.xlsx
+++ b/prisma/seeder/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="132" yWindow="588" windowWidth="22716" windowHeight="8676" activeTab="3"/>
+    <workbookView xWindow="132" yWindow="588" windowWidth="22716" windowHeight="8676" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="account" sheetId="6" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>email</t>
   </si>
@@ -85,18 +85,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>image</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>link</t>
-  </si>
-  <si>
     <t>price</t>
   </si>
   <si>
@@ -118,31 +106,34 @@
     <t>contentTitle</t>
   </si>
   <si>
-    <t>https://via.placeholder.com/150</t>
-  </si>
-  <si>
-    <t>Content 1</t>
-  </si>
-  <si>
-    <t>Content 2</t>
-  </si>
-  <si>
     <t>Video</t>
   </si>
   <si>
     <t>Audio</t>
   </si>
   <si>
-    <t>Description Content 1</t>
-  </si>
-  <si>
-    <t>Description Content 2</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=123456</t>
   </si>
   <si>
     <t>081234567891</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>bunnyId</t>
+  </si>
+  <si>
+    <t>ustadzName</t>
+  </si>
+  <si>
+    <t>Ustadz Hanan Attaki</t>
+  </si>
+  <si>
+    <t>132a4sd6f8as7d9f</t>
+  </si>
+  <si>
+    <t>132a4sd6f8as7d9g</t>
   </si>
 </sst>
 </file>
@@ -557,7 +548,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -637,7 +628,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
@@ -687,7 +678,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
@@ -726,102 +717,94 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>21</v>
       </c>
       <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
       <c r="H1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" t="s">
-        <v>40</v>
+        <v>31</v>
+      </c>
+      <c r="F2">
+        <v>100000</v>
       </c>
       <c r="G2">
-        <v>100000</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
         <v>37</v>
       </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
-      </c>
       <c r="E3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" t="s">
-        <v>40</v>
+        <v>31</v>
+      </c>
+      <c r="F3">
+        <v>100000</v>
       </c>
       <c r="G3">
-        <v>100000</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -834,7 +817,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:C22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -847,28 +832,28 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="str">
-        <f>VLOOKUP(A2,content!A:D,4,0)</f>
-        <v>Content 1</v>
+      <c r="B2" s="4" t="e">
+        <f>VLOOKUP(A2,content!A:C,4,0)</f>
+        <v>#REF!</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -885,9 +870,9 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="str">
-        <f>VLOOKUP(A3,content!A:D,4,0)</f>
-        <v>Content 1</v>
+      <c r="B3" s="4" t="e">
+        <f>VLOOKUP(A3,content!A:C,4,0)</f>
+        <v>#REF!</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -904,9 +889,9 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="str">
-        <f>VLOOKUP(A4,content!A:D,4,0)</f>
-        <v>Content 2</v>
+      <c r="B4" s="4" t="e">
+        <f>VLOOKUP(A4,content!A:C,4,0)</f>
+        <v>#REF!</v>
       </c>
       <c r="C4">
         <v>1</v>

</xml_diff>

<commit_message>
chore: update seeder and add package xlsx and ts-node
</commit_message>
<xml_diff>
--- a/prisma/seeder/data.xlsx
+++ b/prisma/seeder/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="132" yWindow="588" windowWidth="22716" windowHeight="8676" activeTab="3"/>
+    <workbookView xWindow="132" yWindow="588" windowWidth="22716" windowHeight="8676"/>
   </bookViews>
   <sheets>
     <sheet name="account" sheetId="6" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>email</t>
   </si>
@@ -134,6 +134,21 @@
   </si>
   <si>
     <t>Male</t>
+  </si>
+  <si>
+    <t>birthdate</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>Jambi</t>
+  </si>
+  <si>
+    <t>2002-12-03</t>
+  </si>
+  <si>
+    <t>2003-12-03</t>
   </si>
 </sst>
 </file>
@@ -527,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -538,14 +553,16 @@
     <col min="1" max="1" width="2.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="15.69921875" customWidth="1"/>
-    <col min="6" max="6" width="25.5" customWidth="1"/>
-    <col min="7" max="7" width="6.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="13.19921875" customWidth="1"/>
-    <col min="10" max="10" width="8.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="15.69921875" customWidth="1"/>
+    <col min="8" max="8" width="25.5" customWidth="1"/>
+    <col min="9" max="9" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.19921875" customWidth="1"/>
+    <col min="12" max="12" width="8.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -559,25 +576,31 @@
         <v>36</v>
       </c>
       <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -590,26 +613,32 @@
       <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="1">
+      <c r="J2" s="1">
         <v>123456</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="b">
+      <c r="L2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -623,29 +652,35 @@
       <c r="D3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1">
+      <c r="J3" s="1">
         <v>123456</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J3" t="b">
+      <c r="L3" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -807,7 +842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
chore: update schema prisma
</commit_message>
<xml_diff>
--- a/prisma/seeder/data.xlsx
+++ b/prisma/seeder/data.xlsx
@@ -8,16 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="account" sheetId="6" r:id="rId1"/>
-    <sheet name="category" sheetId="7" r:id="rId2"/>
-    <sheet name="content" sheetId="8" r:id="rId3"/>
-    <sheet name="contentCategory" sheetId="9" r:id="rId4"/>
+    <sheet name="ustadz" sheetId="10" r:id="rId2"/>
+    <sheet name="category" sheetId="7" r:id="rId3"/>
+    <sheet name="content" sheetId="8" r:id="rId4"/>
+    <sheet name="contentCategory" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t>email</t>
   </si>
@@ -49,9 +50,6 @@
     <t>isVerified</t>
   </si>
   <si>
-    <t>user@gmail.com</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
@@ -109,9 +107,6 @@
     <t>bunnyId</t>
   </si>
   <si>
-    <t>ustadzName</t>
-  </si>
-  <si>
     <t>Ustadz Hanan Attaki</t>
   </si>
   <si>
@@ -133,12 +128,6 @@
     <t>fullname</t>
   </si>
   <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>birthdate</t>
-  </si>
-  <si>
     <t>city</t>
   </si>
   <si>
@@ -149,6 +138,21 @@
   </si>
   <si>
     <t>2003-12-03</t>
+  </si>
+  <si>
+    <t>fulan@gmail.com</t>
+  </si>
+  <si>
+    <t>birthDate</t>
+  </si>
+  <si>
+    <t>Laki-laki</t>
+  </si>
+  <si>
+    <t>1981-12-31</t>
+  </si>
+  <si>
+    <t>ustadzId</t>
   </si>
 </sst>
 </file>
@@ -545,7 +549,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -564,22 +568,22 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
         <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" t="s">
-        <v>40</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -608,16 +612,16 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>3</v>
@@ -635,7 +639,7 @@
         <v>5</v>
       </c>
       <c r="L2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -644,28 +648,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
         <v>10</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>11</v>
       </c>
       <c r="J3" s="1">
         <v>123456</v>
@@ -687,6 +691,60 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -703,10 +761,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
         <v>8</v>
@@ -717,7 +775,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -729,107 +787,9 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="2.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2">
-        <v>100000</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <f>A2+1</f>
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3">
-        <v>100000</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -839,6 +799,109 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="72.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.8984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.09765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2">
+        <v>100000</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3">
+        <v>100000</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -855,13 +918,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
       <c r="C1" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>